<commit_message>
Deploy Gzhennaxia/Gzhennaxia.github.io to github.com/Gzhennaxia/Gzhennaxia.github.io.git:master
</commit_message>
<xml_diff>
--- a/excel/Abstinence.xlsx
+++ b/excel/Abstinence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gzhennaxia/Documents/GitHub/Gzhennaxia.github.io/source/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD408C2-FDD0-B243-ABED-7232B1151C8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB7F6D9-7533-9D42-92B7-57E076ED8CB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16280" xr2:uid="{7AD4885A-4EC6-B947-B870-264BF5DAC568}"/>
   </bookViews>
@@ -116,8 +116,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="179" formatCode="0.000"/>
+    <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="177" formatCode="0.000"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -235,14 +235,14 @@
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -251,11 +251,7 @@
   <dxfs count="15">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -263,11 +259,10 @@
         <sz val="12"/>
         <color rgb="FF555555"/>
         <name val="等线"/>
-        <family val="4"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="179" formatCode="0.000"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -287,7 +282,27 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="179" formatCode="0.000"/>
+      <numFmt numFmtId="177" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF555555"/>
+        <name val="等线"/>
+        <family val="4"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="177" formatCode="0.000"/>
     </dxf>
     <dxf>
       <font>
@@ -306,7 +321,26 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="176" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <numFmt numFmtId="177" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF555555"/>
+        <name val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="178" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
       <font>
@@ -366,40 +400,6 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF555555"/>
-        <name val="等线"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF555555"/>
-        <name val="等线"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="179" formatCode="0.000"/>
     </dxf>
     <dxf>
       <font>
@@ -563,16 +563,16 @@
       <calculatedColumnFormula>"第 "&amp;WEEKNUM(records[[#This Row],[日期]],2)&amp;" 周"</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="1" xr3:uid="{C122F2B9-2C27-CC49-95C8-A7AF9ECBEB4B}" name="日期" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{C9D28CBA-D9EC-6743-A793-FFD0F93D5C41}" name="Wet-Dream" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{607D6D23-94C7-C441-9805-FA4B15B54167}" name="Porn-Video" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{91709BBD-F72B-4441-AAD6-A9419A8B7AA7}" name="Masturbation" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{C9D28CBA-D9EC-6743-A793-FFD0F93D5C41}" name="Wet-Dream" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{607D6D23-94C7-C441-9805-FA4B15B54167}" name="Porn-Video" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{91709BBD-F72B-4441-AAD6-A9419A8B7AA7}" name="Masturbation" dataDxfId="5">
       <calculatedColumnFormula>records[[#This Row],[Porn-Video]]-records[[#This Row],[Wet-Dream]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D411FE29-4477-0E4A-A7B5-60DC0ABFF15E}" name="Sexual-Intercourse" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{9A7EEC2F-5772-324F-996D-33BE4AEDBF3E}" name="得分" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{D7FBDF7B-DF28-1E47-9775-46452B32D094}" name="正连续天数" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{D411FE29-4477-0E4A-A7B5-60DC0ABFF15E}" name="Sexual-Intercourse" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{9A7EEC2F-5772-324F-996D-33BE4AEDBF3E}" name="得分" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{D7FBDF7B-DF28-1E47-9775-46452B32D094}" name="正连续天数" dataDxfId="2"/>
     <tableColumn id="9" xr3:uid="{4BE38D8D-A385-6F46-83DC-7068208B0366}" name="负连续天数" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{4FB1A93B-C8B6-6540-BFD1-25429D916D4B}" name="备注" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{4FB1A93B-C8B6-6540-BFD1-25429D916D4B}" name="备注" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB9BA94-3697-444E-A1CA-5AFDE3C5B3F6}">
   <dimension ref="A1:Q145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -897,45 +897,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16" customHeight="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:17" ht="23" customHeight="1">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:17" ht="23" customHeight="1">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
     </row>
     <row r="4" spans="1:17" ht="18">
       <c r="A4" s="6" t="s">
@@ -1016,10 +1016,10 @@
       <c r="J5" s="9">
         <v>0.1</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="10">
         <v>1</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="10">
         <v>0</v>
       </c>
       <c r="M5" s="5"/>
@@ -1062,11 +1062,11 @@
       <c r="J6" s="9">
         <v>0.1</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K5+1)</f>
         <v>2</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L5+1, 0)</f>
         <v>0</v>
       </c>
@@ -1110,11 +1110,11 @@
       <c r="J7" s="9">
         <v>0.2</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K6+1)</f>
         <v>3</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L6+1, 0)</f>
         <v>0</v>
       </c>
@@ -1160,11 +1160,11 @@
       <c r="J8" s="9">
         <v>0.2</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K7+1)</f>
         <v>4</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L7+1, 0)</f>
         <v>0</v>
       </c>
@@ -1208,11 +1208,11 @@
       <c r="J9" s="9">
         <v>0.2</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K8+1)</f>
         <v>5</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L8+1, 0)</f>
         <v>0</v>
       </c>
@@ -1256,11 +1256,11 @@
       <c r="J10" s="9">
         <v>0.3</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K9+1)</f>
         <v>6</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L9+1, 0)</f>
         <v>0</v>
       </c>
@@ -1306,11 +1306,11 @@
       <c r="J11" s="9">
         <v>0.5</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K10+1)</f>
         <v>7</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L10+1, 0)</f>
         <v>0</v>
       </c>
@@ -1356,11 +1356,11 @@
       <c r="J12" s="9">
         <v>0.5</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K11+1)</f>
         <v>8</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L11+1, 0)</f>
         <v>0</v>
       </c>
@@ -1404,11 +1404,11 @@
       <c r="J13" s="9">
         <v>0.6</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K12+1)</f>
         <v>9</v>
       </c>
-      <c r="L13" s="11">
+      <c r="L13" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L12+1, 0)</f>
         <v>0</v>
       </c>
@@ -1454,11 +1454,11 @@
       <c r="J14" s="9">
         <v>0.6</v>
       </c>
-      <c r="K14" s="11">
+      <c r="K14" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K13+1)</f>
         <v>10</v>
       </c>
-      <c r="L14" s="11">
+      <c r="L14" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L13+1, 0)</f>
         <v>0</v>
       </c>
@@ -1502,11 +1502,11 @@
       <c r="J15" s="9">
         <v>0.6</v>
       </c>
-      <c r="K15" s="11">
+      <c r="K15" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K14+1)</f>
         <v>11</v>
       </c>
-      <c r="L15" s="11">
+      <c r="L15" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L14+1, 0)</f>
         <v>0</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>43895</v>
       </c>
       <c r="F16" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="5">
         <v>0</v>
@@ -1550,11 +1550,11 @@
       <c r="J16" s="9">
         <v>0.7</v>
       </c>
-      <c r="K16" s="11">
+      <c r="K16" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K15+1)</f>
         <v>12</v>
       </c>
-      <c r="L16" s="11">
+      <c r="L16" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L15+1, 0)</f>
         <v>0</v>
       </c>
@@ -1597,11 +1597,11 @@
       <c r="J17" s="9">
         <v>0.7</v>
       </c>
-      <c r="K17" s="11">
+      <c r="K17" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K16+1)</f>
         <v>13</v>
       </c>
-      <c r="L17" s="11">
+      <c r="L17" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L16+1, 0)</f>
         <v>0</v>
       </c>
@@ -1642,11 +1642,11 @@
       <c r="J18" s="9">
         <v>0.9</v>
       </c>
-      <c r="K18" s="11">
+      <c r="K18" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K17+1)</f>
         <v>14</v>
       </c>
-      <c r="L18" s="11">
+      <c r="L18" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L17+1, 0)</f>
         <v>0</v>
       </c>
@@ -1689,11 +1689,11 @@
       <c r="J19" s="9">
         <v>1</v>
       </c>
-      <c r="K19" s="11">
+      <c r="K19" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K18+1)</f>
         <v>15</v>
       </c>
-      <c r="L19" s="11">
+      <c r="L19" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L18+1, 0)</f>
         <v>0</v>
       </c>
@@ -1736,11 +1736,11 @@
       <c r="J20" s="9">
         <v>1</v>
       </c>
-      <c r="K20" s="11">
+      <c r="K20" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K19+1)</f>
         <v>16</v>
       </c>
-      <c r="L20" s="11">
+      <c r="L20" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L19+1, 0)</f>
         <v>0</v>
       </c>
@@ -1781,11 +1781,11 @@
       <c r="J21" s="9">
         <v>1</v>
       </c>
-      <c r="K21" s="11">
+      <c r="K21" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K20+1)</f>
         <v>17</v>
       </c>
-      <c r="L21" s="11">
+      <c r="L21" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L20+1, 0)</f>
         <v>0</v>
       </c>
@@ -1824,11 +1824,11 @@
         <v>0</v>
       </c>
       <c r="J22" s="9"/>
-      <c r="K22" s="11">
+      <c r="K22" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K21+1)</f>
         <v>18</v>
       </c>
-      <c r="L22" s="11">
+      <c r="L22" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L21+1, 0)</f>
         <v>0</v>
       </c>
@@ -1869,11 +1869,11 @@
         <v>0</v>
       </c>
       <c r="J23" s="9"/>
-      <c r="K23" s="11">
+      <c r="K23" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K22+1)</f>
         <v>19</v>
       </c>
-      <c r="L23" s="11">
+      <c r="L23" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L22+1, 0)</f>
         <v>0</v>
       </c>
@@ -1912,11 +1912,11 @@
         <v>0</v>
       </c>
       <c r="J24" s="9"/>
-      <c r="K24" s="11">
+      <c r="K24" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K23+1)</f>
         <v>20</v>
       </c>
-      <c r="L24" s="11">
+      <c r="L24" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L23+1, 0)</f>
         <v>0</v>
       </c>
@@ -1955,11 +1955,11 @@
         <v>0</v>
       </c>
       <c r="J25" s="9"/>
-      <c r="K25" s="11">
+      <c r="K25" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K24+1)</f>
         <v>21</v>
       </c>
-      <c r="L25" s="11">
+      <c r="L25" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L24+1, 0)</f>
         <v>0</v>
       </c>
@@ -2000,11 +2000,11 @@
         <v>0</v>
       </c>
       <c r="J26" s="9"/>
-      <c r="K26" s="11">
+      <c r="K26" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K25+1)</f>
         <v>22</v>
       </c>
-      <c r="L26" s="11">
+      <c r="L26" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L25+1, 0)</f>
         <v>0</v>
       </c>
@@ -2043,11 +2043,11 @@
         <v>0</v>
       </c>
       <c r="J27" s="9"/>
-      <c r="K27" s="11">
+      <c r="K27" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K26+1)</f>
         <v>23</v>
       </c>
-      <c r="L27" s="11">
+      <c r="L27" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L26+1, 0)</f>
         <v>0</v>
       </c>
@@ -2086,11 +2086,11 @@
         <v>0</v>
       </c>
       <c r="J28" s="9"/>
-      <c r="K28" s="11">
+      <c r="K28" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K27+1)</f>
         <v>24</v>
       </c>
-      <c r="L28" s="11">
+      <c r="L28" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L27+1, 0)</f>
         <v>0</v>
       </c>
@@ -2131,11 +2131,11 @@
         <v>0</v>
       </c>
       <c r="J29" s="9"/>
-      <c r="K29" s="11">
+      <c r="K29" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K28+1)</f>
         <v>25</v>
       </c>
-      <c r="L29" s="11">
+      <c r="L29" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L28+1, 0)</f>
         <v>0</v>
       </c>
@@ -2174,11 +2174,11 @@
         <v>0</v>
       </c>
       <c r="J30" s="9"/>
-      <c r="K30" s="11">
+      <c r="K30" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K29+1)</f>
         <v>26</v>
       </c>
-      <c r="L30" s="11">
+      <c r="L30" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L29+1, 0)</f>
         <v>0</v>
       </c>
@@ -2217,11 +2217,11 @@
         <v>0</v>
       </c>
       <c r="J31" s="9"/>
-      <c r="K31" s="11">
+      <c r="K31" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K30+1)</f>
         <v>27</v>
       </c>
-      <c r="L31" s="11">
+      <c r="L31" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L30+1, 0)</f>
         <v>0</v>
       </c>
@@ -2262,11 +2262,11 @@
         <v>0</v>
       </c>
       <c r="J32" s="9"/>
-      <c r="K32" s="11">
+      <c r="K32" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K31+1)</f>
         <v>28</v>
       </c>
-      <c r="L32" s="11">
+      <c r="L32" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L31+1, 0)</f>
         <v>0</v>
       </c>
@@ -2307,11 +2307,11 @@
         <v>0</v>
       </c>
       <c r="J33" s="9"/>
-      <c r="K33" s="11">
+      <c r="K33" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K32+1)</f>
         <v>29</v>
       </c>
-      <c r="L33" s="11">
+      <c r="L33" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L32+1, 0)</f>
         <v>0</v>
       </c>
@@ -2350,11 +2350,11 @@
         <v>0</v>
       </c>
       <c r="J34" s="9"/>
-      <c r="K34" s="11">
+      <c r="K34" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K33+1)</f>
         <v>30</v>
       </c>
-      <c r="L34" s="11">
+      <c r="L34" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L33+1, 0)</f>
         <v>0</v>
       </c>
@@ -2395,11 +2395,11 @@
         <v>0</v>
       </c>
       <c r="J35" s="9"/>
-      <c r="K35" s="11">
+      <c r="K35" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K34+1)</f>
         <v>31</v>
       </c>
-      <c r="L35" s="11">
+      <c r="L35" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L34+1, 0)</f>
         <v>0</v>
       </c>
@@ -2438,11 +2438,11 @@
         <v>0</v>
       </c>
       <c r="J36" s="9"/>
-      <c r="K36" s="11">
+      <c r="K36" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K35+1)</f>
         <v>32</v>
       </c>
-      <c r="L36" s="11">
+      <c r="L36" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L35+1, 0)</f>
         <v>0</v>
       </c>
@@ -2481,11 +2481,11 @@
         <v>0</v>
       </c>
       <c r="J37" s="9"/>
-      <c r="K37" s="11">
+      <c r="K37" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K36+1)</f>
         <v>33</v>
       </c>
-      <c r="L37" s="11">
+      <c r="L37" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L36+1, 0)</f>
         <v>0</v>
       </c>
@@ -2524,11 +2524,11 @@
         <v>0</v>
       </c>
       <c r="J38" s="9"/>
-      <c r="K38" s="11">
+      <c r="K38" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K37+1)</f>
         <v>34</v>
       </c>
-      <c r="L38" s="11">
+      <c r="L38" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L37+1, 0)</f>
         <v>0</v>
       </c>
@@ -2567,11 +2567,11 @@
         <v>0</v>
       </c>
       <c r="J39" s="9"/>
-      <c r="K39" s="11">
+      <c r="K39" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K38+1)</f>
         <v>35</v>
       </c>
-      <c r="L39" s="11">
+      <c r="L39" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L38+1, 0)</f>
         <v>0</v>
       </c>
@@ -2610,11 +2610,11 @@
         <v>0</v>
       </c>
       <c r="J40" s="9"/>
-      <c r="K40" s="11">
+      <c r="K40" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K39+1)</f>
         <v>36</v>
       </c>
-      <c r="L40" s="11">
+      <c r="L40" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L39+1, 0)</f>
         <v>0</v>
       </c>
@@ -2653,11 +2653,11 @@
         <v>0</v>
       </c>
       <c r="J41" s="9"/>
-      <c r="K41" s="11">
+      <c r="K41" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K40+1)</f>
         <v>37</v>
       </c>
-      <c r="L41" s="11">
+      <c r="L41" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L40+1, 0)</f>
         <v>0</v>
       </c>
@@ -2696,11 +2696,11 @@
         <v>0</v>
       </c>
       <c r="J42" s="9"/>
-      <c r="K42" s="11">
+      <c r="K42" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K41+1)</f>
         <v>38</v>
       </c>
-      <c r="L42" s="11">
+      <c r="L42" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L41+1, 0)</f>
         <v>0</v>
       </c>
@@ -2739,11 +2739,11 @@
         <v>0</v>
       </c>
       <c r="J43" s="9"/>
-      <c r="K43" s="11">
+      <c r="K43" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K42+1)</f>
         <v>39</v>
       </c>
-      <c r="L43" s="11">
+      <c r="L43" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L42+1, 0)</f>
         <v>0</v>
       </c>
@@ -2782,11 +2782,11 @@
         <v>0</v>
       </c>
       <c r="J44" s="9"/>
-      <c r="K44" s="11">
+      <c r="K44" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K43+1)</f>
         <v>40</v>
       </c>
-      <c r="L44" s="11">
+      <c r="L44" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L43+1, 0)</f>
         <v>0</v>
       </c>
@@ -2825,11 +2825,11 @@
         <v>0</v>
       </c>
       <c r="J45" s="9"/>
-      <c r="K45" s="11">
+      <c r="K45" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K44+1)</f>
         <v>41</v>
       </c>
-      <c r="L45" s="11">
+      <c r="L45" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L44+1, 0)</f>
         <v>0</v>
       </c>
@@ -2868,11 +2868,11 @@
         <v>0</v>
       </c>
       <c r="J46" s="9"/>
-      <c r="K46" s="11">
+      <c r="K46" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K45+1)</f>
         <v>42</v>
       </c>
-      <c r="L46" s="11">
+      <c r="L46" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L45+1, 0)</f>
         <v>0</v>
       </c>
@@ -2911,11 +2911,11 @@
         <v>0</v>
       </c>
       <c r="J47" s="9"/>
-      <c r="K47" s="11">
+      <c r="K47" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K46+1)</f>
         <v>43</v>
       </c>
-      <c r="L47" s="11">
+      <c r="L47" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L46+1, 0)</f>
         <v>0</v>
       </c>
@@ -2954,11 +2954,11 @@
         <v>0</v>
       </c>
       <c r="J48" s="9"/>
-      <c r="K48" s="11">
+      <c r="K48" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K47+1)</f>
         <v>44</v>
       </c>
-      <c r="L48" s="11">
+      <c r="L48" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L47+1, 0)</f>
         <v>0</v>
       </c>
@@ -2997,11 +2997,11 @@
         <v>0</v>
       </c>
       <c r="J49" s="9"/>
-      <c r="K49" s="11">
+      <c r="K49" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K48+1)</f>
         <v>45</v>
       </c>
-      <c r="L49" s="11">
+      <c r="L49" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L48+1, 0)</f>
         <v>0</v>
       </c>
@@ -3040,11 +3040,11 @@
         <v>0</v>
       </c>
       <c r="J50" s="9"/>
-      <c r="K50" s="11">
+      <c r="K50" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K49+1)</f>
         <v>46</v>
       </c>
-      <c r="L50" s="11">
+      <c r="L50" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L49+1, 0)</f>
         <v>0</v>
       </c>
@@ -3083,11 +3083,11 @@
         <v>0</v>
       </c>
       <c r="J51" s="9"/>
-      <c r="K51" s="11">
+      <c r="K51" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K50+1)</f>
         <v>47</v>
       </c>
-      <c r="L51" s="11">
+      <c r="L51" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L50+1, 0)</f>
         <v>0</v>
       </c>
@@ -3126,11 +3126,11 @@
         <v>0</v>
       </c>
       <c r="J52" s="9"/>
-      <c r="K52" s="11">
+      <c r="K52" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K51+1)</f>
         <v>48</v>
       </c>
-      <c r="L52" s="11">
+      <c r="L52" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L51+1, 0)</f>
         <v>0</v>
       </c>
@@ -3169,11 +3169,11 @@
         <v>0</v>
       </c>
       <c r="J53" s="9"/>
-      <c r="K53" s="11">
+      <c r="K53" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K52+1)</f>
         <v>49</v>
       </c>
-      <c r="L53" s="11">
+      <c r="L53" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L52+1, 0)</f>
         <v>0</v>
       </c>
@@ -3212,11 +3212,11 @@
         <v>0</v>
       </c>
       <c r="J54" s="9"/>
-      <c r="K54" s="11">
+      <c r="K54" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K53+1)</f>
         <v>50</v>
       </c>
-      <c r="L54" s="11">
+      <c r="L54" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L53+1, 0)</f>
         <v>0</v>
       </c>
@@ -3255,11 +3255,11 @@
         <v>0</v>
       </c>
       <c r="J55" s="9"/>
-      <c r="K55" s="11">
+      <c r="K55" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K54+1)</f>
         <v>51</v>
       </c>
-      <c r="L55" s="11">
+      <c r="L55" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L54+1, 0)</f>
         <v>0</v>
       </c>
@@ -3298,11 +3298,11 @@
         <v>0</v>
       </c>
       <c r="J56" s="9"/>
-      <c r="K56" s="11">
+      <c r="K56" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K55+1)</f>
         <v>52</v>
       </c>
-      <c r="L56" s="11">
+      <c r="L56" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L55+1, 0)</f>
         <v>0</v>
       </c>
@@ -3341,11 +3341,11 @@
         <v>0</v>
       </c>
       <c r="J57" s="9"/>
-      <c r="K57" s="11">
+      <c r="K57" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K56+1)</f>
         <v>53</v>
       </c>
-      <c r="L57" s="11">
+      <c r="L57" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L56+1, 0)</f>
         <v>0</v>
       </c>
@@ -3384,11 +3384,11 @@
         <v>0</v>
       </c>
       <c r="J58" s="9"/>
-      <c r="K58" s="11">
+      <c r="K58" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K57+1)</f>
         <v>54</v>
       </c>
-      <c r="L58" s="11">
+      <c r="L58" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L57+1, 0)</f>
         <v>0</v>
       </c>
@@ -3427,11 +3427,11 @@
         <v>0</v>
       </c>
       <c r="J59" s="9"/>
-      <c r="K59" s="11">
+      <c r="K59" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K58+1)</f>
         <v>55</v>
       </c>
-      <c r="L59" s="11">
+      <c r="L59" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L58+1, 0)</f>
         <v>0</v>
       </c>
@@ -3470,11 +3470,11 @@
         <v>0</v>
       </c>
       <c r="J60" s="9"/>
-      <c r="K60" s="11">
+      <c r="K60" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K59+1)</f>
         <v>56</v>
       </c>
-      <c r="L60" s="11">
+      <c r="L60" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L59+1, 0)</f>
         <v>0</v>
       </c>
@@ -3513,11 +3513,11 @@
         <v>0</v>
       </c>
       <c r="J61" s="9"/>
-      <c r="K61" s="11">
+      <c r="K61" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K60+1)</f>
         <v>57</v>
       </c>
-      <c r="L61" s="11">
+      <c r="L61" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L60+1, 0)</f>
         <v>0</v>
       </c>
@@ -3556,11 +3556,11 @@
         <v>0</v>
       </c>
       <c r="J62" s="9"/>
-      <c r="K62" s="11">
+      <c r="K62" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K61+1)</f>
         <v>58</v>
       </c>
-      <c r="L62" s="11">
+      <c r="L62" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L61+1, 0)</f>
         <v>0</v>
       </c>
@@ -3599,11 +3599,11 @@
         <v>0</v>
       </c>
       <c r="J63" s="9"/>
-      <c r="K63" s="11">
+      <c r="K63" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K62+1)</f>
         <v>59</v>
       </c>
-      <c r="L63" s="11">
+      <c r="L63" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L62+1, 0)</f>
         <v>0</v>
       </c>
@@ -3642,11 +3642,11 @@
         <v>0</v>
       </c>
       <c r="J64" s="9"/>
-      <c r="K64" s="11">
+      <c r="K64" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K63+1)</f>
         <v>60</v>
       </c>
-      <c r="L64" s="11">
+      <c r="L64" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L63+1, 0)</f>
         <v>0</v>
       </c>
@@ -3685,11 +3685,11 @@
         <v>0</v>
       </c>
       <c r="J65" s="9"/>
-      <c r="K65" s="11">
+      <c r="K65" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K64+1)</f>
         <v>61</v>
       </c>
-      <c r="L65" s="11">
+      <c r="L65" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L64+1, 0)</f>
         <v>0</v>
       </c>
@@ -3728,11 +3728,11 @@
         <v>0</v>
       </c>
       <c r="J66" s="9"/>
-      <c r="K66" s="11">
+      <c r="K66" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K65+1)</f>
         <v>62</v>
       </c>
-      <c r="L66" s="11">
+      <c r="L66" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L65+1, 0)</f>
         <v>0</v>
       </c>
@@ -3771,11 +3771,11 @@
         <v>0</v>
       </c>
       <c r="J67" s="9"/>
-      <c r="K67" s="11">
+      <c r="K67" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K66+1)</f>
         <v>63</v>
       </c>
-      <c r="L67" s="11">
+      <c r="L67" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L66+1, 0)</f>
         <v>0</v>
       </c>
@@ -3814,11 +3814,11 @@
         <v>0</v>
       </c>
       <c r="J68" s="9"/>
-      <c r="K68" s="11">
+      <c r="K68" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K67+1)</f>
         <v>64</v>
       </c>
-      <c r="L68" s="11">
+      <c r="L68" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L67+1, 0)</f>
         <v>0</v>
       </c>
@@ -3857,11 +3857,11 @@
         <v>0</v>
       </c>
       <c r="J69" s="9"/>
-      <c r="K69" s="11">
+      <c r="K69" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K68+1)</f>
         <v>65</v>
       </c>
-      <c r="L69" s="11">
+      <c r="L69" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L68+1, 0)</f>
         <v>0</v>
       </c>
@@ -3900,11 +3900,11 @@
         <v>0</v>
       </c>
       <c r="J70" s="9"/>
-      <c r="K70" s="11">
+      <c r="K70" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K69+1)</f>
         <v>66</v>
       </c>
-      <c r="L70" s="11">
+      <c r="L70" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L69+1, 0)</f>
         <v>0</v>
       </c>
@@ -3943,11 +3943,11 @@
         <v>0</v>
       </c>
       <c r="J71" s="9"/>
-      <c r="K71" s="11">
+      <c r="K71" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K70+1)</f>
         <v>67</v>
       </c>
-      <c r="L71" s="11">
+      <c r="L71" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L70+1, 0)</f>
         <v>0</v>
       </c>
@@ -3986,11 +3986,11 @@
         <v>0</v>
       </c>
       <c r="J72" s="9"/>
-      <c r="K72" s="11">
+      <c r="K72" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K71+1)</f>
         <v>68</v>
       </c>
-      <c r="L72" s="11">
+      <c r="L72" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L71+1, 0)</f>
         <v>0</v>
       </c>
@@ -4029,11 +4029,11 @@
         <v>0</v>
       </c>
       <c r="J73" s="9"/>
-      <c r="K73" s="11">
+      <c r="K73" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K72+1)</f>
         <v>69</v>
       </c>
-      <c r="L73" s="11">
+      <c r="L73" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L72+1, 0)</f>
         <v>0</v>
       </c>
@@ -4072,11 +4072,11 @@
         <v>0</v>
       </c>
       <c r="J74" s="9"/>
-      <c r="K74" s="11">
+      <c r="K74" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K73+1)</f>
         <v>70</v>
       </c>
-      <c r="L74" s="11">
+      <c r="L74" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L73+1, 0)</f>
         <v>0</v>
       </c>
@@ -4115,11 +4115,11 @@
         <v>0</v>
       </c>
       <c r="J75" s="9"/>
-      <c r="K75" s="11">
+      <c r="K75" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K74+1)</f>
         <v>71</v>
       </c>
-      <c r="L75" s="11">
+      <c r="L75" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L74+1, 0)</f>
         <v>0</v>
       </c>
@@ -4158,11 +4158,11 @@
         <v>0</v>
       </c>
       <c r="J76" s="9"/>
-      <c r="K76" s="11">
+      <c r="K76" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K75+1)</f>
         <v>72</v>
       </c>
-      <c r="L76" s="11">
+      <c r="L76" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L75+1, 0)</f>
         <v>0</v>
       </c>
@@ -4201,11 +4201,11 @@
         <v>0</v>
       </c>
       <c r="J77" s="9"/>
-      <c r="K77" s="11">
+      <c r="K77" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K76+1)</f>
         <v>73</v>
       </c>
-      <c r="L77" s="11">
+      <c r="L77" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L76+1, 0)</f>
         <v>0</v>
       </c>
@@ -4244,11 +4244,11 @@
         <v>0</v>
       </c>
       <c r="J78" s="9"/>
-      <c r="K78" s="11">
+      <c r="K78" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K77+1)</f>
         <v>74</v>
       </c>
-      <c r="L78" s="11">
+      <c r="L78" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L77+1, 0)</f>
         <v>0</v>
       </c>
@@ -4287,11 +4287,11 @@
         <v>0</v>
       </c>
       <c r="J79" s="9"/>
-      <c r="K79" s="11">
+      <c r="K79" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K78+1)</f>
         <v>75</v>
       </c>
-      <c r="L79" s="11">
+      <c r="L79" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L78+1, 0)</f>
         <v>0</v>
       </c>
@@ -4330,11 +4330,11 @@
         <v>0</v>
       </c>
       <c r="J80" s="9"/>
-      <c r="K80" s="11">
+      <c r="K80" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K79+1)</f>
         <v>76</v>
       </c>
-      <c r="L80" s="11">
+      <c r="L80" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L79+1, 0)</f>
         <v>0</v>
       </c>
@@ -4373,11 +4373,11 @@
         <v>0</v>
       </c>
       <c r="J81" s="9"/>
-      <c r="K81" s="11">
+      <c r="K81" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K80+1)</f>
         <v>77</v>
       </c>
-      <c r="L81" s="11">
+      <c r="L81" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L80+1, 0)</f>
         <v>0</v>
       </c>
@@ -4416,11 +4416,11 @@
         <v>0</v>
       </c>
       <c r="J82" s="9"/>
-      <c r="K82" s="11">
+      <c r="K82" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K81+1)</f>
         <v>78</v>
       </c>
-      <c r="L82" s="11">
+      <c r="L82" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L81+1, 0)</f>
         <v>0</v>
       </c>
@@ -4459,11 +4459,11 @@
         <v>0</v>
       </c>
       <c r="J83" s="9"/>
-      <c r="K83" s="11">
+      <c r="K83" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K82+1)</f>
         <v>79</v>
       </c>
-      <c r="L83" s="11">
+      <c r="L83" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L82+1, 0)</f>
         <v>0</v>
       </c>
@@ -4502,11 +4502,11 @@
         <v>0</v>
       </c>
       <c r="J84" s="9"/>
-      <c r="K84" s="11">
+      <c r="K84" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K83+1)</f>
         <v>80</v>
       </c>
-      <c r="L84" s="11">
+      <c r="L84" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L83+1, 0)</f>
         <v>0</v>
       </c>
@@ -4545,11 +4545,11 @@
         <v>0</v>
       </c>
       <c r="J85" s="9"/>
-      <c r="K85" s="11">
+      <c r="K85" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K84+1)</f>
         <v>81</v>
       </c>
-      <c r="L85" s="11">
+      <c r="L85" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L84+1, 0)</f>
         <v>0</v>
       </c>
@@ -4588,11 +4588,11 @@
         <v>0</v>
       </c>
       <c r="J86" s="9"/>
-      <c r="K86" s="11">
+      <c r="K86" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K85+1)</f>
         <v>82</v>
       </c>
-      <c r="L86" s="11">
+      <c r="L86" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L85+1, 0)</f>
         <v>0</v>
       </c>
@@ -4631,11 +4631,11 @@
         <v>0</v>
       </c>
       <c r="J87" s="9"/>
-      <c r="K87" s="11">
+      <c r="K87" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K86+1)</f>
         <v>83</v>
       </c>
-      <c r="L87" s="11">
+      <c r="L87" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L86+1, 0)</f>
         <v>0</v>
       </c>
@@ -4674,11 +4674,11 @@
         <v>0</v>
       </c>
       <c r="J88" s="9"/>
-      <c r="K88" s="11">
+      <c r="K88" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K87+1)</f>
         <v>84</v>
       </c>
-      <c r="L88" s="11">
+      <c r="L88" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L87+1, 0)</f>
         <v>0</v>
       </c>
@@ -4717,11 +4717,11 @@
         <v>0</v>
       </c>
       <c r="J89" s="9"/>
-      <c r="K89" s="11">
+      <c r="K89" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K88+1)</f>
         <v>85</v>
       </c>
-      <c r="L89" s="11">
+      <c r="L89" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L88+1, 0)</f>
         <v>0</v>
       </c>
@@ -4760,11 +4760,11 @@
         <v>0</v>
       </c>
       <c r="J90" s="9"/>
-      <c r="K90" s="11">
+      <c r="K90" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K89+1)</f>
         <v>86</v>
       </c>
-      <c r="L90" s="11">
+      <c r="L90" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L89+1, 0)</f>
         <v>0</v>
       </c>
@@ -4803,11 +4803,11 @@
         <v>0</v>
       </c>
       <c r="J91" s="9"/>
-      <c r="K91" s="11">
+      <c r="K91" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K90+1)</f>
         <v>87</v>
       </c>
-      <c r="L91" s="11">
+      <c r="L91" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L90+1, 0)</f>
         <v>0</v>
       </c>
@@ -4846,11 +4846,11 @@
         <v>0</v>
       </c>
       <c r="J92" s="9"/>
-      <c r="K92" s="11">
+      <c r="K92" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K91+1)</f>
         <v>88</v>
       </c>
-      <c r="L92" s="11">
+      <c r="L92" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L91+1, 0)</f>
         <v>0</v>
       </c>
@@ -4889,11 +4889,11 @@
         <v>0</v>
       </c>
       <c r="J93" s="9"/>
-      <c r="K93" s="11">
+      <c r="K93" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K92+1)</f>
         <v>89</v>
       </c>
-      <c r="L93" s="11">
+      <c r="L93" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L92+1, 0)</f>
         <v>0</v>
       </c>
@@ -4932,11 +4932,11 @@
         <v>0</v>
       </c>
       <c r="J94" s="9"/>
-      <c r="K94" s="11">
+      <c r="K94" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K93+1)</f>
         <v>90</v>
       </c>
-      <c r="L94" s="11">
+      <c r="L94" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L93+1, 0)</f>
         <v>0</v>
       </c>
@@ -4975,11 +4975,11 @@
         <v>0</v>
       </c>
       <c r="J95" s="9"/>
-      <c r="K95" s="11">
+      <c r="K95" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K94+1)</f>
         <v>91</v>
       </c>
-      <c r="L95" s="11">
+      <c r="L95" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L94+1, 0)</f>
         <v>0</v>
       </c>
@@ -5018,11 +5018,11 @@
         <v>0</v>
       </c>
       <c r="J96" s="9"/>
-      <c r="K96" s="11">
+      <c r="K96" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K95+1)</f>
         <v>92</v>
       </c>
-      <c r="L96" s="11">
+      <c r="L96" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L95+1, 0)</f>
         <v>0</v>
       </c>
@@ -5061,11 +5061,11 @@
         <v>0</v>
       </c>
       <c r="J97" s="9"/>
-      <c r="K97" s="11">
+      <c r="K97" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K96+1)</f>
         <v>93</v>
       </c>
-      <c r="L97" s="11">
+      <c r="L97" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L96+1, 0)</f>
         <v>0</v>
       </c>
@@ -5104,11 +5104,11 @@
         <v>0</v>
       </c>
       <c r="J98" s="9"/>
-      <c r="K98" s="11">
+      <c r="K98" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K97+1)</f>
         <v>94</v>
       </c>
-      <c r="L98" s="11">
+      <c r="L98" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L97+1, 0)</f>
         <v>0</v>
       </c>
@@ -5147,11 +5147,11 @@
         <v>0</v>
       </c>
       <c r="J99" s="9"/>
-      <c r="K99" s="11">
+      <c r="K99" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K98+1)</f>
         <v>95</v>
       </c>
-      <c r="L99" s="11">
+      <c r="L99" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L98+1, 0)</f>
         <v>0</v>
       </c>
@@ -5190,11 +5190,11 @@
         <v>0</v>
       </c>
       <c r="J100" s="9"/>
-      <c r="K100" s="11">
+      <c r="K100" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K99+1)</f>
         <v>96</v>
       </c>
-      <c r="L100" s="11">
+      <c r="L100" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L99+1, 0)</f>
         <v>0</v>
       </c>
@@ -5233,11 +5233,11 @@
         <v>0</v>
       </c>
       <c r="J101" s="9"/>
-      <c r="K101" s="11">
+      <c r="K101" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K100+1)</f>
         <v>97</v>
       </c>
-      <c r="L101" s="11">
+      <c r="L101" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L100+1, 0)</f>
         <v>0</v>
       </c>
@@ -5276,11 +5276,11 @@
         <v>0</v>
       </c>
       <c r="J102" s="9"/>
-      <c r="K102" s="11">
+      <c r="K102" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K101+1)</f>
         <v>98</v>
       </c>
-      <c r="L102" s="11">
+      <c r="L102" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L101+1, 0)</f>
         <v>0</v>
       </c>
@@ -5319,11 +5319,11 @@
         <v>0</v>
       </c>
       <c r="J103" s="9"/>
-      <c r="K103" s="11">
+      <c r="K103" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K102+1)</f>
         <v>99</v>
       </c>
-      <c r="L103" s="11">
+      <c r="L103" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L102+1, 0)</f>
         <v>0</v>
       </c>
@@ -5362,11 +5362,11 @@
         <v>0</v>
       </c>
       <c r="J104" s="9"/>
-      <c r="K104" s="11">
+      <c r="K104" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K103+1)</f>
         <v>100</v>
       </c>
-      <c r="L104" s="11">
+      <c r="L104" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L103+1, 0)</f>
         <v>0</v>
       </c>
@@ -5405,11 +5405,11 @@
         <v>0</v>
       </c>
       <c r="J105" s="9"/>
-      <c r="K105" s="11">
+      <c r="K105" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K104+1)</f>
         <v>101</v>
       </c>
-      <c r="L105" s="11">
+      <c r="L105" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L104+1, 0)</f>
         <v>0</v>
       </c>
@@ -5448,11 +5448,11 @@
         <v>0</v>
       </c>
       <c r="J106" s="9"/>
-      <c r="K106" s="11">
+      <c r="K106" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K105+1)</f>
         <v>102</v>
       </c>
-      <c r="L106" s="11">
+      <c r="L106" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L105+1, 0)</f>
         <v>0</v>
       </c>
@@ -5491,11 +5491,11 @@
         <v>0</v>
       </c>
       <c r="J107" s="9"/>
-      <c r="K107" s="11">
+      <c r="K107" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K106+1)</f>
         <v>103</v>
       </c>
-      <c r="L107" s="11">
+      <c r="L107" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L106+1, 0)</f>
         <v>0</v>
       </c>
@@ -5534,11 +5534,11 @@
         <v>0</v>
       </c>
       <c r="J108" s="9"/>
-      <c r="K108" s="11">
+      <c r="K108" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K107+1)</f>
         <v>104</v>
       </c>
-      <c r="L108" s="11">
+      <c r="L108" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L107+1, 0)</f>
         <v>0</v>
       </c>
@@ -5577,11 +5577,11 @@
         <v>0</v>
       </c>
       <c r="J109" s="9"/>
-      <c r="K109" s="11">
+      <c r="K109" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K108+1)</f>
         <v>105</v>
       </c>
-      <c r="L109" s="11">
+      <c r="L109" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L108+1, 0)</f>
         <v>0</v>
       </c>
@@ -5620,11 +5620,11 @@
         <v>0</v>
       </c>
       <c r="J110" s="9"/>
-      <c r="K110" s="11">
+      <c r="K110" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K109+1)</f>
         <v>106</v>
       </c>
-      <c r="L110" s="11">
+      <c r="L110" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L109+1, 0)</f>
         <v>0</v>
       </c>
@@ -5663,11 +5663,11 @@
         <v>0</v>
       </c>
       <c r="J111" s="9"/>
-      <c r="K111" s="11">
+      <c r="K111" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K110+1)</f>
         <v>107</v>
       </c>
-      <c r="L111" s="11">
+      <c r="L111" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L110+1, 0)</f>
         <v>0</v>
       </c>
@@ -5706,11 +5706,11 @@
         <v>0</v>
       </c>
       <c r="J112" s="9"/>
-      <c r="K112" s="11">
+      <c r="K112" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K111+1)</f>
         <v>108</v>
       </c>
-      <c r="L112" s="11">
+      <c r="L112" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L111+1, 0)</f>
         <v>0</v>
       </c>
@@ -5749,11 +5749,11 @@
         <v>0</v>
       </c>
       <c r="J113" s="9"/>
-      <c r="K113" s="11">
+      <c r="K113" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K112+1)</f>
         <v>109</v>
       </c>
-      <c r="L113" s="11">
+      <c r="L113" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L112+1, 0)</f>
         <v>0</v>
       </c>
@@ -5792,11 +5792,11 @@
         <v>0</v>
       </c>
       <c r="J114" s="9"/>
-      <c r="K114" s="11">
+      <c r="K114" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K113+1)</f>
         <v>110</v>
       </c>
-      <c r="L114" s="11">
+      <c r="L114" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L113+1, 0)</f>
         <v>0</v>
       </c>
@@ -5835,11 +5835,11 @@
         <v>0</v>
       </c>
       <c r="J115" s="9"/>
-      <c r="K115" s="11">
+      <c r="K115" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K114+1)</f>
         <v>111</v>
       </c>
-      <c r="L115" s="11">
+      <c r="L115" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L114+1, 0)</f>
         <v>0</v>
       </c>
@@ -5878,11 +5878,11 @@
         <v>0</v>
       </c>
       <c r="J116" s="9"/>
-      <c r="K116" s="11">
+      <c r="K116" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K115+1)</f>
         <v>112</v>
       </c>
-      <c r="L116" s="11">
+      <c r="L116" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L115+1, 0)</f>
         <v>0</v>
       </c>
@@ -5921,11 +5921,11 @@
         <v>0</v>
       </c>
       <c r="J117" s="9"/>
-      <c r="K117" s="11">
+      <c r="K117" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K116+1)</f>
         <v>113</v>
       </c>
-      <c r="L117" s="11">
+      <c r="L117" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L116+1, 0)</f>
         <v>0</v>
       </c>
@@ -5964,11 +5964,11 @@
         <v>0</v>
       </c>
       <c r="J118" s="9"/>
-      <c r="K118" s="11">
+      <c r="K118" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K117+1)</f>
         <v>114</v>
       </c>
-      <c r="L118" s="11">
+      <c r="L118" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L117+1, 0)</f>
         <v>0</v>
       </c>
@@ -6007,11 +6007,11 @@
         <v>0</v>
       </c>
       <c r="J119" s="9"/>
-      <c r="K119" s="11">
+      <c r="K119" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K118+1)</f>
         <v>115</v>
       </c>
-      <c r="L119" s="11">
+      <c r="L119" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L118+1, 0)</f>
         <v>0</v>
       </c>
@@ -6050,11 +6050,11 @@
         <v>0</v>
       </c>
       <c r="J120" s="9"/>
-      <c r="K120" s="11">
+      <c r="K120" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K119+1)</f>
         <v>116</v>
       </c>
-      <c r="L120" s="11">
+      <c r="L120" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L119+1, 0)</f>
         <v>0</v>
       </c>
@@ -6093,11 +6093,11 @@
         <v>0</v>
       </c>
       <c r="J121" s="9"/>
-      <c r="K121" s="11">
+      <c r="K121" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K120+1)</f>
         <v>117</v>
       </c>
-      <c r="L121" s="11">
+      <c r="L121" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L120+1, 0)</f>
         <v>0</v>
       </c>
@@ -6136,11 +6136,11 @@
         <v>0</v>
       </c>
       <c r="J122" s="9"/>
-      <c r="K122" s="11">
+      <c r="K122" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K121+1)</f>
         <v>118</v>
       </c>
-      <c r="L122" s="11">
+      <c r="L122" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L121+1, 0)</f>
         <v>0</v>
       </c>
@@ -6179,11 +6179,11 @@
         <v>0</v>
       </c>
       <c r="J123" s="9"/>
-      <c r="K123" s="11">
+      <c r="K123" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K122+1)</f>
         <v>119</v>
       </c>
-      <c r="L123" s="11">
+      <c r="L123" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L122+1, 0)</f>
         <v>0</v>
       </c>
@@ -6222,11 +6222,11 @@
         <v>0</v>
       </c>
       <c r="J124" s="9"/>
-      <c r="K124" s="11">
+      <c r="K124" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K123+1)</f>
         <v>120</v>
       </c>
-      <c r="L124" s="11">
+      <c r="L124" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L123+1, 0)</f>
         <v>0</v>
       </c>
@@ -6265,11 +6265,11 @@
         <v>0</v>
       </c>
       <c r="J125" s="9"/>
-      <c r="K125" s="11">
+      <c r="K125" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K124+1)</f>
         <v>121</v>
       </c>
-      <c r="L125" s="11">
+      <c r="L125" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L124+1, 0)</f>
         <v>0</v>
       </c>
@@ -6308,11 +6308,11 @@
         <v>0</v>
       </c>
       <c r="J126" s="9"/>
-      <c r="K126" s="11">
+      <c r="K126" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K125+1)</f>
         <v>122</v>
       </c>
-      <c r="L126" s="11">
+      <c r="L126" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L125+1, 0)</f>
         <v>0</v>
       </c>
@@ -6351,11 +6351,11 @@
         <v>0</v>
       </c>
       <c r="J127" s="9"/>
-      <c r="K127" s="11">
+      <c r="K127" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K126+1)</f>
         <v>123</v>
       </c>
-      <c r="L127" s="11">
+      <c r="L127" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L126+1, 0)</f>
         <v>0</v>
       </c>
@@ -6394,11 +6394,11 @@
         <v>0</v>
       </c>
       <c r="J128" s="9"/>
-      <c r="K128" s="11">
+      <c r="K128" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K127+1)</f>
         <v>124</v>
       </c>
-      <c r="L128" s="11">
+      <c r="L128" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L127+1, 0)</f>
         <v>0</v>
       </c>
@@ -6437,11 +6437,11 @@
         <v>0</v>
       </c>
       <c r="J129" s="9"/>
-      <c r="K129" s="11">
+      <c r="K129" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K128+1)</f>
         <v>125</v>
       </c>
-      <c r="L129" s="11">
+      <c r="L129" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L128+1, 0)</f>
         <v>0</v>
       </c>
@@ -6480,11 +6480,11 @@
         <v>0</v>
       </c>
       <c r="J130" s="9"/>
-      <c r="K130" s="11">
+      <c r="K130" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K129+1)</f>
         <v>126</v>
       </c>
-      <c r="L130" s="11">
+      <c r="L130" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L129+1, 0)</f>
         <v>0</v>
       </c>
@@ -6523,11 +6523,11 @@
         <v>0</v>
       </c>
       <c r="J131" s="9"/>
-      <c r="K131" s="11">
+      <c r="K131" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K130+1)</f>
         <v>127</v>
       </c>
-      <c r="L131" s="11">
+      <c r="L131" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L130+1, 0)</f>
         <v>0</v>
       </c>
@@ -6566,11 +6566,11 @@
         <v>0</v>
       </c>
       <c r="J132" s="9"/>
-      <c r="K132" s="11">
+      <c r="K132" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K131+1)</f>
         <v>128</v>
       </c>
-      <c r="L132" s="11">
+      <c r="L132" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L131+1, 0)</f>
         <v>0</v>
       </c>
@@ -6609,11 +6609,11 @@
         <v>0</v>
       </c>
       <c r="J133" s="9"/>
-      <c r="K133" s="11">
+      <c r="K133" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K132+1)</f>
         <v>129</v>
       </c>
-      <c r="L133" s="11">
+      <c r="L133" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L132+1, 0)</f>
         <v>0</v>
       </c>
@@ -6652,11 +6652,11 @@
         <v>0</v>
       </c>
       <c r="J134" s="9"/>
-      <c r="K134" s="11">
+      <c r="K134" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K133+1)</f>
         <v>130</v>
       </c>
-      <c r="L134" s="11">
+      <c r="L134" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L133+1, 0)</f>
         <v>0</v>
       </c>
@@ -6695,11 +6695,11 @@
         <v>0</v>
       </c>
       <c r="J135" s="9"/>
-      <c r="K135" s="11">
+      <c r="K135" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K134+1)</f>
         <v>131</v>
       </c>
-      <c r="L135" s="11">
+      <c r="L135" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L134+1, 0)</f>
         <v>0</v>
       </c>
@@ -6738,11 +6738,11 @@
         <v>0</v>
       </c>
       <c r="J136" s="9"/>
-      <c r="K136" s="11">
+      <c r="K136" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K135+1)</f>
         <v>132</v>
       </c>
-      <c r="L136" s="11">
+      <c r="L136" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L135+1, 0)</f>
         <v>0</v>
       </c>
@@ -6781,11 +6781,11 @@
         <v>0</v>
       </c>
       <c r="J137" s="9"/>
-      <c r="K137" s="11">
+      <c r="K137" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K136+1)</f>
         <v>133</v>
       </c>
-      <c r="L137" s="11">
+      <c r="L137" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L136+1, 0)</f>
         <v>0</v>
       </c>
@@ -6824,11 +6824,11 @@
         <v>0</v>
       </c>
       <c r="J138" s="9"/>
-      <c r="K138" s="11">
+      <c r="K138" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K137+1)</f>
         <v>134</v>
       </c>
-      <c r="L138" s="11">
+      <c r="L138" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L137+1, 0)</f>
         <v>0</v>
       </c>
@@ -6867,11 +6867,11 @@
         <v>0</v>
       </c>
       <c r="J139" s="9"/>
-      <c r="K139" s="11">
+      <c r="K139" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K138+1)</f>
         <v>135</v>
       </c>
-      <c r="L139" s="11">
+      <c r="L139" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L138+1, 0)</f>
         <v>0</v>
       </c>
@@ -6910,11 +6910,11 @@
         <v>0</v>
       </c>
       <c r="J140" s="9"/>
-      <c r="K140" s="11">
+      <c r="K140" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K139+1)</f>
         <v>136</v>
       </c>
-      <c r="L140" s="11">
+      <c r="L140" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L139+1, 0)</f>
         <v>0</v>
       </c>
@@ -6953,11 +6953,11 @@
         <v>0</v>
       </c>
       <c r="J141" s="9"/>
-      <c r="K141" s="11">
+      <c r="K141" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K140+1)</f>
         <v>137</v>
       </c>
-      <c r="L141" s="11">
+      <c r="L141" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L140+1, 0)</f>
         <v>0</v>
       </c>
@@ -6996,11 +6996,11 @@
         <v>0</v>
       </c>
       <c r="J142" s="9"/>
-      <c r="K142" s="11">
+      <c r="K142" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K141+1)</f>
         <v>138</v>
       </c>
-      <c r="L142" s="11">
+      <c r="L142" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L141+1, 0)</f>
         <v>0</v>
       </c>
@@ -7039,11 +7039,11 @@
         <v>0</v>
       </c>
       <c r="J143" s="9"/>
-      <c r="K143" s="11">
+      <c r="K143" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K142+1)</f>
         <v>139</v>
       </c>
-      <c r="L143" s="11">
+      <c r="L143" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L142+1, 0)</f>
         <v>0</v>
       </c>
@@ -7082,11 +7082,11 @@
         <v>0</v>
       </c>
       <c r="J144" s="9"/>
-      <c r="K144" s="11">
+      <c r="K144" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K143+1)</f>
         <v>140</v>
       </c>
-      <c r="L144" s="11">
+      <c r="L144" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L143+1, 0)</f>
         <v>0</v>
       </c>
@@ -7125,11 +7125,11 @@
         <v>0</v>
       </c>
       <c r="J145" s="9"/>
-      <c r="K145" s="11">
+      <c r="K145" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), 0, K144+1)</f>
         <v>141</v>
       </c>
-      <c r="L145" s="11">
+      <c r="L145" s="10">
         <f>IF(((records[Porn-Video]+records[Masturbation]+records[Sexual-Intercourse])&gt;0), L144+1, 0)</f>
         <v>0</v>
       </c>

</xml_diff>